<commit_message>
Update ESD protection block
</commit_message>
<xml_diff>
--- a/BOM_v2.xlsx
+++ b/BOM_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebburton/Documents/GitHub/Low-Cost_EEG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F7C601-BEB4-044D-9075-AE3F5C7032E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F9E2AD-690D-4D42-9FBF-2C01DA589D20}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,7 +445,7 @@
     <t>C6, C8, C9, C10, C13, C14, C20, C23, C26, C28, C31, C34, C35</t>
   </si>
   <si>
-    <t>D3, D4, D5, D6, D7, D8, D9, D10</t>
+    <t>D3, D4, D5, D6, D7, D8, D9, D10, D11, D12</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -533,12 +533,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,7 +560,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -580,9 +574,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -592,7 +583,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1052,7 +1042,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1121,7 +1111,7 @@
         <f t="shared" ref="A3:A20" si="0">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>139</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -1139,7 +1129,7 @@
       <c r="G3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>14</v>
       </c>
       <c r="I3" s="10">
@@ -1155,7 +1145,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>140</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -1207,7 +1197,7 @@
       <c r="G5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <v>1</v>
       </c>
       <c r="I5" s="10">
@@ -1326,7 +1316,7 @@
       <c r="B9" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>89</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -1341,7 +1331,7 @@
       <c r="G9" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <v>1</v>
       </c>
       <c r="I9" s="10">
@@ -1459,7 +1449,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="7" t="s">
         <v>117</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -1601,16 +1591,16 @@
       <c r="C17" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>36</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>108</v>
       </c>
       <c r="H17" s="8">
@@ -1632,10 +1622,10 @@
       <c r="B18" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="8" t="s">
@@ -1644,7 +1634,7 @@
       <c r="F18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="15" t="s">
         <v>104</v>
       </c>
       <c r="H18" s="8">
@@ -1666,7 +1656,7 @@
       <c r="B19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="8" t="s">
@@ -1678,7 +1668,7 @@
       <c r="F19" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="15" t="s">
         <v>67</v>
       </c>
       <c r="H19" s="8">
@@ -1712,7 +1702,7 @@
       <c r="F20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="15" t="s">
         <v>69</v>
       </c>
       <c r="H20" s="8">
@@ -1728,13 +1718,13 @@
     </row>
     <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <f>A20+1</f>
+        <f t="shared" ref="A21:A34" si="3">A20+1</f>
         <v>20</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="8" t="s">
@@ -1746,24 +1736,24 @@
       <c r="F21" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="18" t="str">
+      <c r="G21" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/on-semiconductor/1N5234BTR/1N5234BFSCT-ND/3504334")</f>
         <v>https://www.digikey.com/product-detail/en/on-semiconductor/1N5234BTR/1N5234BFSCT-ND/3504334</v>
       </c>
       <c r="H21" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I21" s="10">
         <v>0.121</v>
       </c>
       <c r="J21" s="10">
         <f>I21*H21</f>
-        <v>0.96799999999999997</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <f>A21+1</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1781,7 +1771,7 @@
       <c r="F22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="18" t="str">
+      <c r="G22" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/panasonic-electronic-components/EVQ-11U04M/P8082SCT-ND/259567")</f>
         <v>https://www.digikey.com/product-detail/en/panasonic-electronic-components/EVQ-11U04M/P8082SCT-ND/259567</v>
       </c>
@@ -1798,7 +1788,7 @@
     </row>
     <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <f>A22+1</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1807,7 +1797,7 @@
       <c r="C23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E23" s="8" t="s">
@@ -1816,7 +1806,7 @@
       <c r="F23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="18" t="str">
+      <c r="G23" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/e-switch/EG1218/EG1903-ND/101726")</f>
         <v>https://www.digikey.com/product-detail/en/e-switch/EG1218/EG1903-ND/101726</v>
       </c>
@@ -1833,13 +1823,13 @@
     </row>
     <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <f>A23+1</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -1851,7 +1841,7 @@
       <c r="F24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="18" t="str">
+      <c r="G24" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/microchip-technology/MCP4921-E-P/MCP4921-E-P-ND/716280")</f>
         <v>https://www.digikey.com/product-detail/en/microchip-technology/MCP4921-E-P/MCP4921-E-P-ND/716280</v>
       </c>
@@ -1868,13 +1858,13 @@
     </row>
     <row r="25" spans="1:10" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <f>A24+1</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="18" t="s">
         <v>36</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -1883,33 +1873,33 @@
       <c r="E25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="16" t="str">
+      <c r="G25" s="15" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/texas-instruments/TL972IP/296-34316-5-ND/1906129")</f>
         <v>https://www.digikey.com/product-detail/en/texas-instruments/TL972IP/296-34316-5-ND/1906129</v>
       </c>
       <c r="H25" s="7">
         <v>1</v>
       </c>
-      <c r="I25" s="22">
+      <c r="I25" s="20">
         <v>0.84</v>
       </c>
-      <c r="J25" s="22">
+      <c r="J25" s="20">
         <f>I25*H25</f>
         <v>0.84</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <f>A25+1</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="8" t="s">
@@ -1921,7 +1911,7 @@
       <c r="F26" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="18" t="str">
+      <c r="G26" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/microchip-technology/TC7650CPA/TC7650CPA-ND/115291")</f>
         <v>https://www.digikey.com/product-detail/en/microchip-technology/TC7650CPA/TC7650CPA-ND/115291</v>
       </c>
@@ -1938,13 +1928,13 @@
     </row>
     <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <f>A26+1</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="8" t="s">
@@ -1956,7 +1946,7 @@
       <c r="F27" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="18" t="str">
+      <c r="G27" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/texas-instruments/CD40107BE/296-3504-5-ND/376603")</f>
         <v>https://www.digikey.com/product-detail/en/texas-instruments/CD40107BE/296-3504-5-ND/376603</v>
       </c>
@@ -1973,13 +1963,13 @@
     </row>
     <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <f>A27+1</f>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="8" t="s">
@@ -1991,7 +1981,7 @@
       <c r="F28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="18" t="str">
+      <c r="G28" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/analog-devices-inc/AD627ANZ/AD627ANZ-ND/750980")</f>
         <v>https://www.digikey.com/product-detail/en/analog-devices-inc/AD627ANZ/AD627ANZ-ND/750980</v>
       </c>
@@ -2008,13 +1998,13 @@
     </row>
     <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
-        <f>A28+1</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="8" t="s">
@@ -2026,7 +2016,7 @@
       <c r="F29" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="18" t="str">
+      <c r="G29" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/linear-technology-analog-devices/LTC1152CN8-PBF/LTC1152CN8-PBF-ND/891149")</f>
         <v>https://www.digikey.com/product-detail/en/linear-technology-analog-devices/LTC1152CN8-PBF/LTC1152CN8-PBF-ND/891149</v>
       </c>
@@ -2043,13 +2033,13 @@
     </row>
     <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
-        <f>A29+1</f>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D30" s="8" t="s">
@@ -2061,7 +2051,7 @@
       <c r="F30" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="18" t="str">
+      <c r="G30" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/microchip-technology/MCP6002-I-P/MCP6002-I-P-ND/500875")</f>
         <v>https://www.digikey.com/product-detail/en/microchip-technology/MCP6002-I-P/MCP6002-I-P-ND/500875</v>
       </c>
@@ -2078,13 +2068,13 @@
     </row>
     <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <f>A30+1</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D31" s="8" t="s">
@@ -2096,7 +2086,7 @@
       <c r="F31" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G31" s="16" t="s">
         <v>83</v>
       </c>
       <c r="H31" s="8">
@@ -2111,14 +2101,14 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="23">
-        <f>A31+1</f>
+      <c r="A32" s="21">
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -2130,7 +2120,7 @@
       <c r="F32" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="16" t="s">
         <v>73</v>
       </c>
       <c r="H32" s="8">
@@ -2145,14 +2135,14 @@
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="23">
-        <f>A32+1</f>
+      <c r="A33" s="21">
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="18" t="s">
         <v>36</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -2161,33 +2151,33 @@
       <c r="E33" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G33" s="16" t="str">
+      <c r="G33" s="15" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/texas-instruments/TS12A4514P/296-21908-5-ND/1629081")</f>
         <v>https://www.digikey.com/product-detail/en/texas-instruments/TS12A4514P/296-21908-5-ND/1629081</v>
       </c>
       <c r="H33" s="7">
         <v>3</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I33" s="20">
         <v>0.76</v>
       </c>
-      <c r="J33" s="22">
+      <c r="J33" s="20">
         <f>I33*H33</f>
         <v>2.2800000000000002</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="23">
-        <f>A33+1</f>
+      <c r="A34" s="21">
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="18" t="s">
         <v>36</v>
       </c>
       <c r="D34" s="7" t="s">
@@ -2196,27 +2186,27 @@
       <c r="E34" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="F34" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G34" s="16" t="str">
+      <c r="G34" s="15" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/sparkfun-electronics/BOB-00544/1568-1345-ND/5824094")</f>
         <v>https://www.digikey.com/product-detail/en/sparkfun-electronics/BOB-00544/1568-1345-ND/5824094</v>
       </c>
       <c r="H34" s="7">
         <v>1</v>
       </c>
-      <c r="I34" s="22">
+      <c r="I34" s="20">
         <v>3.95</v>
       </c>
-      <c r="J34" s="22">
+      <c r="J34" s="20">
         <f>I34*H34</f>
         <v>3.95</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
-        <f t="shared" ref="A25:A38" si="3">A34+1</f>
+        <f t="shared" ref="A35:A38" si="4">A34+1</f>
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
@@ -2234,7 +2224,7 @@
       <c r="F35" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G35" s="18" t="str">
+      <c r="G35" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/texas-instruments/TPS7230QP/296-1965-5-ND")</f>
         <v>https://www.digikey.com/product-detail/en/texas-instruments/TPS7230QP/296-1965-5-ND</v>
       </c>
@@ -2251,13 +2241,13 @@
     </row>
     <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D36" s="8" t="s">
@@ -2269,7 +2259,7 @@
       <c r="F36" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G36" s="18" t="s">
+      <c r="G36" s="16" t="s">
         <v>71</v>
       </c>
       <c r="H36" s="8">
@@ -2285,13 +2275,13 @@
     </row>
     <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D37" s="8" t="s">
@@ -2303,7 +2293,7 @@
       <c r="F37" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G37" s="18" t="str">
+      <c r="G37" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/texas-instruments/UCC3946N/296-11547-5-ND/381725")</f>
         <v>https://www.digikey.com/product-detail/en/texas-instruments/UCC3946N/296-11547-5-ND/381725</v>
       </c>
@@ -2320,7 +2310,7 @@
     </row>
     <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -2338,7 +2328,7 @@
       <c r="F38" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G38" s="18" t="str">
+      <c r="G38" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/ecs-inc/ECS-32-17-1X/X980-ND/827472")</f>
         <v>https://www.digikey.com/product-detail/en/ecs-inc/ECS-32-17-1X/X980-ND/827472</v>
       </c>
@@ -2354,18 +2344,18 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="25">
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="23">
         <f>SUM(J5:J38)</f>
-        <v>95.048000000000002</v>
+        <v>95.29</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="13" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Fixed typo in BOM
</commit_message>
<xml_diff>
--- a/BOM_v2.xlsx
+++ b/BOM_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebburton/Documents/GitHub/Low-Cost_EEG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F9E2AD-690D-4D42-9FBF-2C01DA589D20}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7310F448-5BAB-1241-BFC6-1E73D49786F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1022,9 +1022,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1234,7 +1234,9 @@
       <c r="H6" s="8">
         <v>2</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
       <c r="J6" s="10">
         <f>I6*H6</f>
         <v>0</v>

</xml_diff>

<commit_message>
Update instrumentation amps with DIP replacements
</commit_message>
<xml_diff>
--- a/BOM_v2.xlsx
+++ b/BOM_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebburton/Documents/GitHub/Low-Cost_EEG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7310F448-5BAB-1241-BFC6-1E73D49786F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8045AC-124C-1844-A8B3-18AC9B3A77AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>Resistor 1k</t>
   </si>
   <si>
-    <t>Resistor 2k</t>
-  </si>
-  <si>
     <t>Resistor 10k</t>
   </si>
   <si>
@@ -319,9 +316,6 @@
     <t>1 kΩ</t>
   </si>
   <si>
-    <t>2 kΩ</t>
-  </si>
-  <si>
     <t>10 kΩ</t>
   </si>
   <si>
@@ -373,9 +367,6 @@
     <t>R10, R11, R18, R19, R31</t>
   </si>
   <si>
-    <t>R6, R7, R12, R15, R16, R23, R24, R25, R28, R29</t>
-  </si>
-  <si>
     <t>B1 (a)</t>
   </si>
   <si>
@@ -446,6 +437,15 @@
   </si>
   <si>
     <t>D3, D4, D5, D6, D7, D8, D9, D10, D11, D12</t>
+  </si>
+  <si>
+    <t>5 kΩ</t>
+  </si>
+  <si>
+    <t>Resistor 5k</t>
+  </si>
+  <si>
+    <t>R6, R7, R12, R23, R24, R25, R28, R29</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -588,9 +588,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1022,9 +1019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1042,11 +1039,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -1058,19 +1055,19 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1078,22 +1075,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H2" s="8">
         <v>2</v>
@@ -1108,26 +1105,26 @@
     </row>
     <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
-        <f t="shared" ref="A3:A20" si="0">A2+1</f>
+        <f t="shared" ref="A3:A38" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" s="11">
         <v>14</v>
@@ -1146,22 +1143,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H4" s="8">
         <v>13</v>
@@ -1180,22 +1177,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H5" s="11">
         <v>1</v>
@@ -1214,22 +1211,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H6" s="8">
         <v>2</v>
@@ -1248,22 +1245,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7" s="8">
         <v>1</v>
@@ -1282,22 +1279,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H8" s="8">
         <v>3</v>
@@ -1315,32 +1312,32 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>89</v>
+      <c r="B9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="11">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="H9" s="8">
+        <v>4</v>
       </c>
       <c r="I9" s="10">
         <v>0</v>
       </c>
       <c r="J9" s="10">
-        <f t="shared" si="1"/>
+        <f>I9*H9</f>
         <v>0</v>
       </c>
     </row>
@@ -1349,32 +1346,32 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>116</v>
+      <c r="B10" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I10" s="10">
         <v>0</v>
       </c>
       <c r="J10" s="10">
-        <f t="shared" si="1"/>
+        <f>I10*H10</f>
         <v>0</v>
       </c>
     </row>
@@ -1384,25 +1381,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>99</v>
+        <v>112</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="8">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="H11" s="11">
+        <v>1</v>
       </c>
       <c r="I11" s="10">
         <v>0</v>
@@ -1418,31 +1415,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H12" s="8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I12" s="10">
         <v>0</v>
       </c>
       <c r="J12" s="10">
-        <f t="shared" si="1"/>
+        <f>I12*H12</f>
         <v>0</v>
       </c>
     </row>
@@ -1451,32 +1448,32 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>117</v>
+      <c r="B13" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" s="8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I13" s="10">
         <v>0</v>
       </c>
       <c r="J13" s="10">
-        <f t="shared" si="1"/>
+        <f>I13*H13</f>
         <v>0</v>
       </c>
     </row>
@@ -1485,26 +1482,26 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>112</v>
+      <c r="B14" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H14" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I14" s="10">
         <v>0</v>
@@ -1519,23 +1516,23 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>111</v>
+      <c r="B15" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" s="8">
         <v>2</v>
@@ -1553,26 +1550,26 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>110</v>
+      <c r="B16" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I16" s="10">
         <v>0</v>
@@ -1588,22 +1585,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="G17" s="15" t="s">
         <v>106</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>108</v>
       </c>
       <c r="H17" s="8">
         <v>1</v>
@@ -1618,26 +1615,26 @@
     </row>
     <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G18" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H18" s="8">
         <v>1</v>
@@ -1656,22 +1653,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="F19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="15" t="s">
         <v>66</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>67</v>
       </c>
       <c r="H19" s="8">
         <v>1</v>
@@ -1690,22 +1687,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="F20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="H20" s="8">
         <v>1</v>
@@ -1720,23 +1717,23 @@
     </row>
     <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <f t="shared" ref="A21:A34" si="3">A20+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G21" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/on-semiconductor/1N5234BTR/1N5234BFSCT-ND/3504334")</f>
@@ -1755,23 +1752,23 @@
     </row>
     <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G22" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/panasonic-electronic-components/EVQ-11U04M/P8082SCT-ND/259567")</f>
@@ -1790,23 +1787,23 @@
     </row>
     <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G23" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/e-switch/EG1218/EG1903-ND/101726")</f>
@@ -1825,23 +1822,23 @@
     </row>
     <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G24" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/microchip-technology/MCP4921-E-P/MCP4921-E-P-ND/716280")</f>
@@ -1860,23 +1857,23 @@
     </row>
     <row r="25" spans="1:10" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G25" s="15" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/texas-instruments/TL972IP/296-34316-5-ND/1906129")</f>
@@ -1895,23 +1892,23 @@
     </row>
     <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G26" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/microchip-technology/TC7650CPA/TC7650CPA-ND/115291")</f>
@@ -1930,23 +1927,23 @@
     </row>
     <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G27" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/texas-instruments/CD40107BE/296-3504-5-ND/376603")</f>
@@ -1965,23 +1962,23 @@
     </row>
     <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G28" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/analog-devices-inc/AD627ANZ/AD627ANZ-ND/750980")</f>
@@ -2000,23 +1997,23 @@
     </row>
     <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G29" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/linear-technology-analog-devices/LTC1152CN8-PBF/LTC1152CN8-PBF-ND/891149")</f>
@@ -2035,23 +2032,23 @@
     </row>
     <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G30" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/microchip-technology/MCP6002-I-P/MCP6002-I-P-ND/500875")</f>
@@ -2070,26 +2067,26 @@
     </row>
     <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F31" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" s="16" t="s">
         <v>82</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>83</v>
       </c>
       <c r="H31" s="8">
         <v>1</v>
@@ -2103,27 +2100,27 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="21">
-        <f t="shared" si="3"/>
+      <c r="A32" s="6">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>73</v>
       </c>
       <c r="H32" s="8">
         <v>1</v>
@@ -2137,24 +2134,24 @@
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="21">
-        <f t="shared" si="3"/>
+      <c r="A33" s="6">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G33" s="15" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/texas-instruments/TS12A4514P/296-21908-5-ND/1629081")</f>
@@ -2172,24 +2169,24 @@
       </c>
     </row>
     <row r="34" spans="1:10" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="21">
-        <f t="shared" si="3"/>
+      <c r="A34" s="6">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G34" s="15" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/sparkfun-electronics/BOB-00544/1568-1345-ND/5824094")</f>
@@ -2208,23 +2205,23 @@
     </row>
     <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
-        <f t="shared" ref="A35:A38" si="4">A34+1</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C35" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="F35" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G35" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/texas-instruments/TPS7230QP/296-1965-5-ND")</f>
@@ -2243,26 +2240,26 @@
     </row>
     <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F36" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>71</v>
       </c>
       <c r="H36" s="8">
         <v>1</v>
@@ -2277,23 +2274,23 @@
     </row>
     <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G37" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/texas-instruments/UCC3946N/296-11547-5-ND/381725")</f>
@@ -2312,23 +2309,23 @@
     </row>
     <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="F38" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G38" s="16" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/ecs-inc/ECS-32-17-1X/X980-ND/827472")</f>
@@ -2346,16 +2343,16 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="23">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="22">
         <f>SUM(J5:J38)</f>
         <v>95.29</v>
       </c>

</xml_diff>

<commit_message>
Remove two unnecessary bypass capacitors
</commit_message>
<xml_diff>
--- a/BOM_v2.xlsx
+++ b/BOM_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebburton/Documents/GitHub/Low-Cost_EEG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8045AC-124C-1844-A8B3-18AC9B3A77AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE97C939-9166-E948-A268-D3809122C3E4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,12 +430,6 @@
     <t>C22, C27, C36</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C12, C15, C18, C21, C24, C25, C29, C30, C32, C33</t>
-  </si>
-  <si>
-    <t>C6, C8, C9, C10, C13, C14, C20, C23, C26, C28, C31, C34, C35</t>
-  </si>
-  <si>
     <t>D3, D4, D5, D6, D7, D8, D9, D10, D11, D12</t>
   </si>
   <si>
@@ -446,6 +440,12 @@
   </si>
   <si>
     <t>R6, R7, R12, R23, R24, R25, R28, R29</t>
+  </si>
+  <si>
+    <t>C6, C8, C9, C10, C13, C14, C20, C23, C26, C28, C34</t>
+  </si>
+  <si>
+    <t>C2, C3, C4, C5, C12, C15, C18, C21, C24, C25, C29, C32</t>
   </si>
 </sst>
 </file>
@@ -1020,14 +1020,14 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
@@ -1109,7 +1109,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>93</v>
@@ -1127,7 +1127,7 @@
         <v>64</v>
       </c>
       <c r="H3" s="11">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I3" s="10">
         <v>0</v>
@@ -1143,7 +1143,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>92</v>
@@ -1161,7 +1161,7 @@
         <v>64</v>
       </c>
       <c r="H4" s="8">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I4" s="10">
         <v>0</v>
@@ -1415,7 +1415,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>99</v>
@@ -1520,13 +1520,13 @@
         <v>113</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>64</v>
@@ -1721,7 +1721,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>35</v>

</xml_diff>